<commit_message>
Added the product sheet
</commit_message>
<xml_diff>
--- a/jumia.xlsx
+++ b/jumia.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Sql Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="125">
   <si>
     <t>id</t>
   </si>
@@ -348,6 +348,63 @@
   </si>
   <si>
     <t>subcategory</t>
+  </si>
+  <si>
+    <t>Sid01</t>
+  </si>
+  <si>
+    <t>Sid02</t>
+  </si>
+  <si>
+    <t>Sid03</t>
+  </si>
+  <si>
+    <t>Sid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tvs </t>
+  </si>
+  <si>
+    <t>Sid16</t>
+  </si>
+  <si>
+    <t>Sid04</t>
+  </si>
+  <si>
+    <t>Sid05</t>
+  </si>
+  <si>
+    <t>Sid06</t>
+  </si>
+  <si>
+    <t>Sid08</t>
+  </si>
+  <si>
+    <t>Sid09</t>
+  </si>
+  <si>
+    <t>Household Items</t>
+  </si>
+  <si>
+    <t>Sid11</t>
+  </si>
+  <si>
+    <t>Sid13</t>
+  </si>
+  <si>
+    <t>Sid07</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Clothes</t>
+  </si>
+  <si>
+    <t>Sid10</t>
+  </si>
+  <si>
+    <t>_+</t>
   </si>
 </sst>
 </file>
@@ -383,9 +440,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,10 +818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,127 +842,234 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
       <c r="C2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
       <c r="C3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
       <c r="C4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
       <c r="C6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
       <c r="C7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
       <c r="C8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
       <c r="C9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
       <c r="C10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
         <v>73</v>
       </c>
     </row>
@@ -911,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,6 +1153,11 @@
       </c>
       <c r="B8" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1113,15 +1287,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1131,16 +1306,16 @@
       <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1151,14 +1326,17 @@
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>150</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>200</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1168,11 +1346,17 @@
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>20000</v>
       </c>
-      <c r="E3">
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
         <v>50</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1182,11 +1366,17 @@
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>400</v>
       </c>
-      <c r="E4">
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1">
         <v>87</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1196,11 +1386,17 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>2000</v>
       </c>
-      <c r="E5">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
         <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1210,11 +1406,17 @@
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>800</v>
       </c>
-      <c r="E6">
+      <c r="D6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="1">
         <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1224,11 +1426,17 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>600</v>
       </c>
-      <c r="E7">
+      <c r="D7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="1">
         <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1238,11 +1446,17 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>530</v>
       </c>
-      <c r="E8">
+      <c r="D8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1">
         <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1252,11 +1466,17 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>70</v>
       </c>
-      <c r="E9">
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1">
         <v>65</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,11 +1486,17 @@
       <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>835</v>
       </c>
-      <c r="E10">
+      <c r="D10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="1">
         <v>28</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1280,11 +1506,17 @@
       <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>1200</v>
       </c>
-      <c r="E11">
+      <c r="D11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="1">
         <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>